<commit_message>
python + AI en Excel
</commit_message>
<xml_diff>
--- a/9. Power Query & Pivot/Caso Carvajal/Listado de Agentes.xlsx
+++ b/9. Power Query & Pivot/Caso Carvajal/Listado de Agentes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28706"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,7 +15,23 @@
   <sheets>
     <sheet name="Agentes de TI" sheetId="12" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -30,325 +46,325 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
+    <t>Agentes Carvajal</t>
+  </si>
+  <si>
+    <t>Fecha de nacimiento</t>
+  </si>
+  <si>
+    <t>ID Agente</t>
+  </si>
+  <si>
     <t>Nombre</t>
   </si>
   <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Año</t>
+  </si>
+  <si>
+    <t>Mes</t>
+  </si>
+  <si>
+    <t>Día</t>
+  </si>
+  <si>
+    <t>Mata Lucero</t>
+  </si>
+  <si>
+    <t>lucero.mata@carvajal.com</t>
+  </si>
+  <si>
+    <t>JesusGrajeda</t>
+  </si>
+  <si>
+    <t>jesus.grajeda@carvajal.com</t>
+  </si>
+  <si>
     <t>Elena Velez</t>
   </si>
   <si>
+    <t>elena.velez@carvajal.com</t>
+  </si>
+  <si>
+    <t>Barraza Alberto</t>
+  </si>
+  <si>
+    <t>alberto.barraza@carvajal.com</t>
+  </si>
+  <si>
+    <t>Willyberto Gonzales</t>
+  </si>
+  <si>
+    <t>willyberto.gonzales@carvajal.com</t>
+  </si>
+  <si>
+    <t>A. Trejo</t>
+  </si>
+  <si>
+    <t>alberto.trejo@carvajal.com</t>
+  </si>
+  <si>
     <t>Estuardo Ocaño</t>
   </si>
   <si>
+    <t>estuardo.ocaño@carvajal.com</t>
+  </si>
+  <si>
     <t>Marisol Piedrahita</t>
   </si>
   <si>
+    <t>marisol.piedrahita@carvajal.com</t>
+  </si>
+  <si>
+    <t>Velasquez Jose</t>
+  </si>
+  <si>
+    <t>jose.velasquez@carvajal.com</t>
+  </si>
+  <si>
     <t>Alberto Casillas</t>
   </si>
   <si>
+    <t>alberto.casillas@carvajal.com</t>
+  </si>
+  <si>
+    <t>Lopez Moran.</t>
+  </si>
+  <si>
+    <t>lopez.moran@carvajal.com</t>
+  </si>
+  <si>
+    <t>Javier D.</t>
+  </si>
+  <si>
+    <t>javier.davila@carvajal.com</t>
+  </si>
+  <si>
     <t>Griselda Galindo</t>
   </si>
   <si>
+    <t>griselda.galindo@carvajal.com</t>
+  </si>
+  <si>
+    <t>EstuardoTorres</t>
+  </si>
+  <si>
+    <t>estuardo.torres@carvajal.com</t>
+  </si>
+  <si>
+    <t>Galindo Guadalupe</t>
+  </si>
+  <si>
+    <t>guadalupe.galindo@carvajal.com</t>
+  </si>
+  <si>
+    <t>Orci Carlos</t>
+  </si>
+  <si>
+    <t>carlos.orci@carvajal.com</t>
+  </si>
+  <si>
+    <t>Leon Lourdes</t>
+  </si>
+  <si>
+    <t>lourdes.leon@carvajal.com</t>
+  </si>
+  <si>
     <t>Miller Gaviria</t>
   </si>
   <si>
+    <t>miller.gaviria@carvajal.com</t>
+  </si>
+  <si>
     <t>Alfonso Barraza</t>
   </si>
   <si>
+    <t>alfonso.barraza@carvajal.com</t>
+  </si>
+  <si>
     <t>Eduardo Luna</t>
   </si>
   <si>
+    <t>eduardo.luna@carvajal.com</t>
+  </si>
+  <si>
     <t>Alberto Gastelum</t>
   </si>
   <si>
+    <t>alberto.gastelum@carvajal.com</t>
+  </si>
+  <si>
+    <t>Lorena</t>
+  </si>
+  <si>
+    <t>lorena.leon@carvajal.com</t>
+  </si>
+  <si>
     <t>Guadalupe Hernandez</t>
   </si>
   <si>
+    <t>guadalupe.hernandez@carvajal.com</t>
+  </si>
+  <si>
     <t>Barbara Grijalva</t>
   </si>
   <si>
+    <t>barbara.grijalva@carvajal.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sandra Lujan </t>
   </si>
   <si>
+    <t>sandra.lujan@carvajal.com</t>
+  </si>
+  <si>
     <t>Flores Sierra</t>
   </si>
   <si>
+    <t>flores.sierra@carvajal.com</t>
+  </si>
+  <si>
     <t>Isela Leyva</t>
   </si>
   <si>
+    <t>isela.leyva@carvajal.com</t>
+  </si>
+  <si>
+    <t>Nurio Zepeda</t>
+  </si>
+  <si>
+    <t>nurio.zepeda@carvajal.com</t>
+  </si>
+  <si>
     <t>Segura Garcia</t>
   </si>
   <si>
+    <t>segura.garcia@carvajal.com</t>
+  </si>
+  <si>
     <t>Parra Luna</t>
   </si>
   <si>
+    <t>parra.luna@carvajal.com</t>
+  </si>
+  <si>
     <t>Guadalupe Torrico</t>
   </si>
   <si>
+    <t>guadalupe.torrico@carvajal.com</t>
+  </si>
+  <si>
     <t>Silvia Morales</t>
   </si>
   <si>
+    <t>silvia.morales@carvajal.com</t>
+  </si>
+  <si>
     <t>Guadalupe Villanueva</t>
   </si>
   <si>
+    <t>guadalupe.villanueva@carvajal.com</t>
+  </si>
+  <si>
     <t>Diana Rojo</t>
   </si>
   <si>
+    <t>diana.rojo@carvajal.com</t>
+  </si>
+  <si>
+    <t>Melinda</t>
+  </si>
+  <si>
+    <t>melinda.barcelo@carvajal.com</t>
+  </si>
+  <si>
     <t>Luis Torres</t>
   </si>
   <si>
+    <t>luis.torres@carvajal.com</t>
+  </si>
+  <si>
     <t>Jesus Pacheco</t>
   </si>
   <si>
+    <t>jesus.pacheco@carvajal.com</t>
+  </si>
+  <si>
     <t>Enrique Montiel</t>
   </si>
   <si>
+    <t>enrique.montiel@carvajal.com</t>
+  </si>
+  <si>
     <t>Jesus Contreras</t>
   </si>
   <si>
+    <t>jesus.contreras@carvajal.com</t>
+  </si>
+  <si>
     <t>Alfredo Barreras</t>
   </si>
   <si>
+    <t>alfredo.barreras@carvajal.com</t>
+  </si>
+  <si>
     <t>Aldo Carrillo</t>
   </si>
   <si>
+    <t>aldo.carrillo@carvajal.com</t>
+  </si>
+  <si>
+    <t>Darwin E.</t>
+  </si>
+  <si>
+    <t>darwin.echeverry@carvajal.com</t>
+  </si>
+  <si>
     <t>Reyna Santacruz</t>
   </si>
   <si>
+    <t>reyna.santacruz@carvajal.com</t>
+  </si>
+  <si>
     <t>Eva Cardenas</t>
   </si>
   <si>
+    <t>eva.cardenas@carvajal.com</t>
+  </si>
+  <si>
     <t>Luis Arguello</t>
   </si>
   <si>
+    <t>luis.arguello@carvajal.com</t>
+  </si>
+  <si>
     <t>Rosa Olguin</t>
   </si>
   <si>
+    <t>rosa.olguin@carvajal.com</t>
+  </si>
+  <si>
     <t>Yomaira Agudelo</t>
   </si>
   <si>
+    <t>yomaira.agudelo@carvajal.com</t>
+  </si>
+  <si>
+    <t>Aurelio Tanori</t>
+  </si>
+  <si>
+    <t>aurelio.tanori@carvajal.com</t>
+  </si>
+  <si>
     <t>Armando Sierra</t>
   </si>
   <si>
+    <t>armando.sierra@carvajal.com</t>
+  </si>
+  <si>
     <t>Ramon Macias</t>
-  </si>
-  <si>
-    <t>ID Agente</t>
-  </si>
-  <si>
-    <t>Año</t>
-  </si>
-  <si>
-    <t>Mes</t>
-  </si>
-  <si>
-    <t>Día</t>
-  </si>
-  <si>
-    <t>Fecha de nacimiento</t>
-  </si>
-  <si>
-    <t>Aurelio Tanori</t>
-  </si>
-  <si>
-    <t>Willyberto Gonzales</t>
-  </si>
-  <si>
-    <t>Nurio Zepeda</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>Lorena</t>
-  </si>
-  <si>
-    <t>Melinda</t>
-  </si>
-  <si>
-    <t>Mata Lucero</t>
-  </si>
-  <si>
-    <t>Barraza Alberto</t>
-  </si>
-  <si>
-    <t>Velasquez Jose</t>
-  </si>
-  <si>
-    <t>Galindo Guadalupe</t>
-  </si>
-  <si>
-    <t>Orci Carlos</t>
-  </si>
-  <si>
-    <t>Leon Lourdes</t>
-  </si>
-  <si>
-    <t>A. Trejo</t>
-  </si>
-  <si>
-    <t>Javier D.</t>
-  </si>
-  <si>
-    <t>EstuardoTorres</t>
-  </si>
-  <si>
-    <t>JesusGrajeda</t>
-  </si>
-  <si>
-    <t>Darwin E.</t>
-  </si>
-  <si>
-    <t>Lopez Moran.</t>
-  </si>
-  <si>
-    <t>Agentes Carvajal</t>
-  </si>
-  <si>
-    <t>lucero.mata@carvajal.com</t>
-  </si>
-  <si>
-    <t>jesus.grajeda@carvajal.com</t>
-  </si>
-  <si>
-    <t>elena.velez@carvajal.com</t>
-  </si>
-  <si>
-    <t>alberto.barraza@carvajal.com</t>
-  </si>
-  <si>
-    <t>willyberto.gonzales@carvajal.com</t>
-  </si>
-  <si>
-    <t>alberto.trejo@carvajal.com</t>
-  </si>
-  <si>
-    <t>estuardo.ocaño@carvajal.com</t>
-  </si>
-  <si>
-    <t>marisol.piedrahita@carvajal.com</t>
-  </si>
-  <si>
-    <t>jose.velasquez@carvajal.com</t>
-  </si>
-  <si>
-    <t>alberto.casillas@carvajal.com</t>
-  </si>
-  <si>
-    <t>lopez.moran@carvajal.com</t>
-  </si>
-  <si>
-    <t>javier.davila@carvajal.com</t>
-  </si>
-  <si>
-    <t>griselda.galindo@carvajal.com</t>
-  </si>
-  <si>
-    <t>estuardo.torres@carvajal.com</t>
-  </si>
-  <si>
-    <t>guadalupe.galindo@carvajal.com</t>
-  </si>
-  <si>
-    <t>carlos.orci@carvajal.com</t>
-  </si>
-  <si>
-    <t>lourdes.leon@carvajal.com</t>
-  </si>
-  <si>
-    <t>miller.gaviria@carvajal.com</t>
-  </si>
-  <si>
-    <t>alfonso.barraza@carvajal.com</t>
-  </si>
-  <si>
-    <t>eduardo.luna@carvajal.com</t>
-  </si>
-  <si>
-    <t>alberto.gastelum@carvajal.com</t>
-  </si>
-  <si>
-    <t>lorena.leon@carvajal.com</t>
-  </si>
-  <si>
-    <t>guadalupe.hernandez@carvajal.com</t>
-  </si>
-  <si>
-    <t>barbara.grijalva@carvajal.com</t>
-  </si>
-  <si>
-    <t>sandra.lujan@carvajal.com</t>
-  </si>
-  <si>
-    <t>flores.sierra@carvajal.com</t>
-  </si>
-  <si>
-    <t>isela.leyva@carvajal.com</t>
-  </si>
-  <si>
-    <t>nurio.zepeda@carvajal.com</t>
-  </si>
-  <si>
-    <t>segura.garcia@carvajal.com</t>
-  </si>
-  <si>
-    <t>parra.luna@carvajal.com</t>
-  </si>
-  <si>
-    <t>guadalupe.torrico@carvajal.com</t>
-  </si>
-  <si>
-    <t>silvia.morales@carvajal.com</t>
-  </si>
-  <si>
-    <t>guadalupe.villanueva@carvajal.com</t>
-  </si>
-  <si>
-    <t>diana.rojo@carvajal.com</t>
-  </si>
-  <si>
-    <t>melinda.barcelo@carvajal.com</t>
-  </si>
-  <si>
-    <t>luis.torres@carvajal.com</t>
-  </si>
-  <si>
-    <t>jesus.pacheco@carvajal.com</t>
-  </si>
-  <si>
-    <t>enrique.montiel@carvajal.com</t>
-  </si>
-  <si>
-    <t>jesus.contreras@carvajal.com</t>
-  </si>
-  <si>
-    <t>alfredo.barreras@carvajal.com</t>
-  </si>
-  <si>
-    <t>aldo.carrillo@carvajal.com</t>
-  </si>
-  <si>
-    <t>darwin.echeverry@carvajal.com</t>
-  </si>
-  <si>
-    <t>reyna.santacruz@carvajal.com</t>
-  </si>
-  <si>
-    <t>eva.cardenas@carvajal.com</t>
-  </si>
-  <si>
-    <t>luis.arguello@carvajal.com</t>
-  </si>
-  <si>
-    <t>rosa.olguin@carvajal.com</t>
-  </si>
-  <si>
-    <t>yomaira.agudelo@carvajal.com</t>
-  </si>
-  <si>
-    <t>aurelio.tanori@carvajal.com</t>
-  </si>
-  <si>
-    <t>armando.sierra@carvajal.com</t>
   </si>
   <si>
     <t>ramon.macias@carvajal.com</t>
@@ -358,7 +374,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -904,11 +920,11 @@
     <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1238,55 +1254,55 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.6">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1">
         <v>1989</v>
@@ -1298,15 +1314,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1">
         <v>1979</v>
@@ -1318,15 +1334,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1">
         <v>1993</v>
@@ -1338,15 +1354,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1">
         <v>1978</v>
@@ -1358,15 +1374,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1">
         <v>1973</v>
@@ -1378,15 +1394,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1">
         <v>1988</v>
@@ -1398,15 +1414,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="D9" s="1">
         <v>1980</v>
@@ -1418,15 +1434,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="D10" s="1">
         <v>1993</v>
@@ -1438,15 +1454,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="D11" s="1">
         <v>1981</v>
@@ -1458,15 +1474,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="D12" s="1">
         <v>1993</v>
@@ -1478,15 +1494,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1">
         <v>1980</v>
@@ -1498,15 +1514,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="D14" s="1">
         <v>1976</v>
@@ -1518,15 +1534,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="D15" s="1">
         <v>1996</v>
@@ -1538,15 +1554,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="D16" s="1">
         <v>1995</v>
@@ -1558,15 +1574,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="D17" s="1">
         <v>1995</v>
@@ -1578,15 +1594,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="D18" s="1">
         <v>1982</v>
@@ -1598,15 +1614,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="D19" s="1">
         <v>1971</v>
@@ -1618,15 +1634,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="D20" s="1">
         <v>1980</v>
@@ -1638,15 +1654,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="D21" s="1">
         <v>1990</v>
@@ -1658,15 +1674,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="D22" s="1">
         <v>1983</v>
@@ -1678,15 +1694,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="D23" s="1">
         <v>1996</v>
@@ -1698,15 +1714,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="D24" s="1">
         <v>1996</v>
@@ -1718,15 +1734,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="D25" s="1">
         <v>1986</v>
@@ -1738,15 +1754,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="D26" s="1">
         <v>1972</v>
@@ -1758,15 +1774,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="D27" s="1">
         <v>1988</v>
@@ -1778,15 +1794,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="D28" s="1">
         <v>1982</v>
@@ -1798,15 +1814,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="D29" s="1">
         <v>1987</v>
@@ -1818,15 +1834,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="D30" s="1">
         <v>1982</v>
@@ -1838,15 +1854,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="D31" s="1">
         <v>1972</v>
@@ -1858,15 +1874,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="D32" s="1">
         <v>1995</v>
@@ -1878,15 +1894,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="D33" s="1">
         <v>1993</v>
@@ -1898,15 +1914,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="D34" s="1">
         <v>1980</v>
@@ -1918,15 +1934,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="D35" s="1">
         <v>1975</v>
@@ -1938,15 +1954,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="D36" s="1">
         <v>1996</v>
@@ -1958,15 +1974,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="D37" s="1">
         <v>1996</v>
@@ -1978,15 +1994,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="D38" s="1">
         <v>1982</v>
@@ -1998,15 +2014,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>22</v>
+        <v>80</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="D39" s="1">
         <v>1980</v>
@@ -2018,15 +2034,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="D40" s="1">
         <v>1985</v>
@@ -2038,15 +2054,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="D41" s="1">
         <v>1983</v>
@@ -2058,15 +2074,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D42" s="1">
         <v>1974</v>
@@ -2078,15 +2094,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D43" s="1">
         <v>1982</v>
@@ -2098,15 +2114,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D44" s="1">
         <v>1991</v>
@@ -2118,15 +2134,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>27</v>
+        <v>92</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D45" s="1">
         <v>1984</v>
@@ -2138,15 +2154,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>28</v>
+        <v>94</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D46" s="1">
         <v>1987</v>
@@ -2158,15 +2174,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D47" s="1">
         <v>1982</v>
@@ -2178,15 +2194,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D48" s="1">
         <v>1985</v>
@@ -2198,15 +2214,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>31</v>
+        <v>100</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D49" s="1">
         <v>1974</v>
@@ -2218,15 +2234,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D50" s="1">
         <v>1979</v>
@@ -2238,15 +2254,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>32</v>
+        <v>104</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D51" s="1">
         <v>1991</v>
@@ -2258,12 +2274,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6">
       <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>107</v>
@@ -2278,8 +2294,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B53" s="4"/>
+    <row r="53" spans="1:6">
+      <c r="B53" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2295,9 +2311,5 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40265564-ABFE-495E-B29A-0D28AD76EB89}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/DataMashup"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40265564-ABFE-495E-B29A-0D28AD76EB89}"/>
 </file>
</xml_diff>